<commit_message>
[Update] circle assemby code
</commit_message>
<xml_diff>
--- a/Docs/ISA Reference sheet.xlsx
+++ b/Docs/ISA Reference sheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\TEC\II-2023\Arquitectura de computadores II\VectorArchitecture\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5B7640-29BE-49DD-8A5F-7B41948050A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58A9DE9-84B7-4BA9-9B81-9CE3D9AD03B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F87682CF-2300-4068-A9F8-89F4A5C197C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11520" activeTab="1" xr2:uid="{F87682CF-2300-4068-A9F8-89F4A5C197C4}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="2" r:id="rId1"/>
-    <sheet name="Codificacion" sheetId="1" r:id="rId2"/>
-    <sheet name="Instrucciones" sheetId="3" r:id="rId3"/>
+    <sheet name="ISA v2" sheetId="4" r:id="rId2"/>
+    <sheet name="Codificacion" sheetId="1" r:id="rId3"/>
+    <sheet name="Instrucciones" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="176">
   <si>
     <t>Bit numbers:</t>
   </si>
@@ -510,17 +511,89 @@
   </si>
   <si>
     <t>VR15</t>
+  </si>
+  <si>
+    <t>movi r0, 90; sum r1, r0, r0</t>
+  </si>
+  <si>
+    <t>r5 = 230</t>
+  </si>
+  <si>
+    <t>loadv VR4, r5</t>
+  </si>
+  <si>
+    <t>mem[i, i+1,]</t>
+  </si>
+  <si>
+    <t>mov VR4[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregar </t>
+  </si>
+  <si>
+    <t>bit de isVector</t>
+  </si>
+  <si>
+    <t>indice de vector</t>
+  </si>
+  <si>
+    <t>INSTRUCCIONES DE DATOS VECTORIALES</t>
+  </si>
+  <si>
+    <t>vsum</t>
+  </si>
+  <si>
+    <t>vres</t>
+  </si>
+  <si>
+    <t>vmul</t>
+  </si>
+  <si>
+    <t>vcmp</t>
+  </si>
+  <si>
+    <t>INSTRUCCIONES DE MEMORIA VECTORIAL</t>
+  </si>
+  <si>
+    <t>vcrg</t>
+  </si>
+  <si>
+    <t>vesc</t>
+  </si>
+  <si>
+    <t>INDEX[2:0]</t>
+  </si>
+  <si>
+    <t>FREE[7:5]</t>
+  </si>
+  <si>
+    <t>vmov</t>
+  </si>
+  <si>
+    <t>isVector[4:3]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="22"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -686,7 +759,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -807,243 +880,276 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="11" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1067,15 +1173,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3255819</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
+      <xdr:colOff>2235283</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>268432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>588819</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>26082</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>724890</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>121332</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1098,8 +1204,57 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13438910" y="7100455"/>
-          <a:ext cx="5004954" cy="3316536"/>
+          <a:off x="12331783" y="5901789"/>
+          <a:ext cx="4966607" cy="3390757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>692729</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>294408</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1318966</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>255546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82AE2177-99E1-425C-A07C-871AB080A9C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12330547" y="5836226"/>
+          <a:ext cx="4990419" cy="3424775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1408,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D974F3-CC49-40D8-BCB6-3C240C833F46}">
-  <dimension ref="A1:L699"/>
+  <dimension ref="A1:M699"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView topLeftCell="A19" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G33" sqref="A12:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27.75" x14ac:dyDescent="0.4"/>
@@ -1423,7 +1578,8 @@
     <col min="5" max="5" width="10.85546875" style="42"/>
     <col min="6" max="7" width="10.85546875" style="43"/>
     <col min="8" max="8" width="24.78515625" style="47" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="32"/>
+    <col min="10" max="10" width="13" style="32" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
@@ -1451,14 +1607,14 @@
       <c r="H1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72" t="s">
+      <c r="J1" s="73"/>
+      <c r="K1" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="72"/>
+      <c r="L1" s="73"/>
     </row>
     <row r="2" spans="1:12" ht="38.25" x14ac:dyDescent="0.4">
       <c r="A2" s="60" t="s">
@@ -1508,12 +1664,12 @@
       <c r="C3" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
       <c r="H3" s="46"/>
       <c r="I3" s="34" t="s">
         <v>94</v>
@@ -1646,12 +1802,12 @@
       <c r="C7" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
       <c r="H7" s="46"/>
       <c r="I7" s="34" t="s">
         <v>99</v>
@@ -1797,15 +1953,15 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
       <c r="H12" s="46"/>
       <c r="I12" s="34" t="s">
         <v>104</v>
@@ -1842,7 +1998,9 @@
       <c r="G13" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="70"/>
+      <c r="H13" s="70" t="s">
+        <v>156</v>
+      </c>
       <c r="I13" s="34" t="s">
         <v>105</v>
       </c>
@@ -2080,12 +2238,12 @@
       <c r="C21" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="76" t="s">
+      <c r="D21" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
       <c r="H21" s="46" t="s">
         <v>131</v>
       </c>
@@ -2113,15 +2271,15 @@
       <c r="J22" s="37"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
       <c r="H23" s="46"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
@@ -2197,15 +2355,15 @@
       <c r="H27" s="46"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
       <c r="H28" s="46"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.4">
@@ -2216,12 +2374,12 @@
       <c r="C29" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="71" t="s">
+      <c r="D29" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
       <c r="H29" s="46"/>
     </row>
     <row r="30" spans="1:12" ht="38.25" x14ac:dyDescent="0.4">
@@ -2232,31 +2390,42 @@
         <v>1011</v>
       </c>
       <c r="C30" s="50"/>
-      <c r="D30" s="71" t="s">
+      <c r="D30" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
       <c r="H30" s="46" t="s">
         <v>128</v>
       </c>
+      <c r="I30" t="s">
+        <v>161</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="K30" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="71" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="49">
         <v>1101</v>
       </c>
       <c r="C31" s="50"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
       <c r="H31" s="46" t="s">
         <v>134</v>
       </c>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
     </row>
     <row r="32" spans="1:12" ht="38.25" x14ac:dyDescent="0.4">
       <c r="A32" s="48" t="s">
@@ -2266,15 +2435,15 @@
         <v>1111</v>
       </c>
       <c r="C32" s="50"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
       <c r="H32" s="46" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="48" t="s">
         <v>66</v>
       </c>
@@ -2292,7 +2461,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34"/>
       <c r="B34" s="32"/>
       <c r="C34"/>
@@ -2300,8 +2469,11 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35"/>
       <c r="B35" s="32"/>
       <c r="C35"/>
@@ -2309,8 +2481,11 @@
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H35" s="47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36"/>
       <c r="B36" s="32"/>
       <c r="C36"/>
@@ -2318,8 +2493,11 @@
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H36" s="47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37"/>
       <c r="B37" s="32"/>
       <c r="C37"/>
@@ -2327,8 +2505,11 @@
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H37" s="47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38"/>
       <c r="B38" s="32"/>
       <c r="C38"/>
@@ -2336,8 +2517,11 @@
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H38" s="47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39"/>
       <c r="B39" s="32"/>
       <c r="C39"/>
@@ -2346,7 +2530,7 @@
       <c r="F39"/>
       <c r="G39"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40"/>
       <c r="B40" s="32"/>
       <c r="C40"/>
@@ -2355,7 +2539,7 @@
       <c r="F40"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41"/>
       <c r="B41" s="32"/>
       <c r="C41"/>
@@ -2364,7 +2548,7 @@
       <c r="F41"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42"/>
       <c r="B42" s="32"/>
       <c r="C42"/>
@@ -2373,7 +2557,7 @@
       <c r="F42"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43"/>
       <c r="B43" s="32"/>
       <c r="C43"/>
@@ -2382,7 +2566,7 @@
       <c r="F43"/>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44"/>
       <c r="B44" s="32"/>
       <c r="C44"/>
@@ -2391,7 +2575,7 @@
       <c r="F44"/>
       <c r="G44"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45"/>
       <c r="B45" s="32"/>
       <c r="C45"/>
@@ -2400,7 +2584,7 @@
       <c r="F45"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46"/>
       <c r="B46" s="32"/>
       <c r="C46"/>
@@ -2409,7 +2593,7 @@
       <c r="F46"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47"/>
       <c r="B47" s="32"/>
       <c r="C47"/>
@@ -2418,7 +2602,7 @@
       <c r="F47"/>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48"/>
       <c r="B48" s="32"/>
       <c r="C48"/>
@@ -8299,7 +8483,7 @@
     <mergeCell ref="D21:G21"/>
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="B14:B15" numberStoredAsText="1"/>
@@ -8309,6 +8493,601 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A16D2C-0E12-4829-A9C3-C55B96002CD1}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="27.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A1" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="88" t="s">
+        <v>173</v>
+      </c>
+      <c r="N2" s="88" t="s">
+        <v>175</v>
+      </c>
+      <c r="O2" s="88" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A3" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="86" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="86" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="49">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="86" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="49">
+        <v>1000</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="49">
+        <v>1001</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="86" t="s">
+        <v>168</v>
+      </c>
+      <c r="I8" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="55"/>
+      <c r="K8" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="57"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="86" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="57"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="92"/>
+      <c r="M10" s="92"/>
+      <c r="N10" s="92"/>
+      <c r="O10" s="92"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="52"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="89" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="48"/>
+      <c r="I13" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="M13" s="88" t="s">
+        <v>173</v>
+      </c>
+      <c r="N13" s="88" t="s">
+        <v>175</v>
+      </c>
+      <c r="O13" s="88" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="K14" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="52"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A15" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="55"/>
+      <c r="K15" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="L15" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="48"/>
+      <c r="B18" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="49">
+        <v>1011</v>
+      </c>
+      <c r="C19" s="50"/>
+      <c r="D19" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="49">
+        <v>1101</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="49">
+        <v>1111</v>
+      </c>
+      <c r="C21" s="50"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="49">
+        <v>1100</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="H12:O12"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A317AB03-9AA6-4FE4-B635-6861460B6D61}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -8374,12 +9153,12 @@
       <c r="C3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="82"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
@@ -8460,12 +9239,12 @@
       <c r="C7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="22" t="s">
@@ -8545,7 +9324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E419E45A-2786-4144-86CB-D6F20170503C}">
   <dimension ref="A1:F15"/>
   <sheetViews>

</xml_diff>